<commit_message>
Ajout des fp et des w
</commit_message>
<xml_diff>
--- a/cordes/delta_f.xlsx
+++ b/cordes/delta_f.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lxqse\Documents\ATIAM\TP-Acoustique-ATIAM\cordes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3116DC15-FCF7-405A-8F2F-DC6014CDB3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94042609-B575-42FC-A8A6-80B49F6A1970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{137D3F44-2C5E-4772-A809-CEACBA3D6FD5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
   <si>
     <t>f-</t>
   </si>
@@ -81,6 +81,36 @@
   </si>
   <si>
     <t>Ukulele 28g</t>
+  </si>
+  <si>
+    <t>dw-</t>
+  </si>
+  <si>
+    <t>dwh</t>
+  </si>
+  <si>
+    <t>dwf+</t>
+  </si>
+  <si>
+    <t>w-</t>
+  </si>
+  <si>
+    <t>wh</t>
+  </si>
+  <si>
+    <t>wf+</t>
+  </si>
+  <si>
+    <t>fp</t>
+  </si>
+  <si>
+    <t>wp</t>
+  </si>
+  <si>
+    <t>dfp</t>
+  </si>
+  <si>
+    <t>dwp</t>
   </si>
 </sst>
 </file>
@@ -432,10 +462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C3003E5-8D39-48AF-8FD5-FF37A8978EE0}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +473,7 @@
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -462,8 +492,38 @@
       <c r="G1" t="s">
         <v>7</v>
       </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -488,8 +548,48 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="H2">
+        <f>B2 * 2 * PI()</f>
+        <v>650.30967929308713</v>
+      </c>
+      <c r="I2">
+        <f>C2 * 2 * PI()</f>
+        <v>772.8317927830891</v>
+      </c>
+      <c r="J2">
+        <f>D2 * 2 * PI()</f>
+        <v>1256.6370614359173</v>
+      </c>
+      <c r="K2">
+        <f>E2 * 2 * PI()</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f>F2 * 2 * PI()</f>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f>G2 * 2 * PI()</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f>SQRT(D2*D2+B2*B2-C2*C2)</f>
+        <v>188.63523000754657</v>
+      </c>
+      <c r="O2">
+        <f>N2*2*PI()</f>
+        <v>1185.2301055998585</v>
+      </c>
+      <c r="P2">
+        <f>$N$2-N2</f>
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <f>P2*2*PI()</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -514,8 +614,48 @@
         <f t="shared" ref="G3:G5" si="2">D$2-D3</f>
         <v>4.6999999999999886</v>
       </c>
+      <c r="H3">
+        <f>B3 * 2 * PI()</f>
+        <v>564.23004058472679</v>
+      </c>
+      <c r="I3">
+        <f>C3 * 2 * PI()</f>
+        <v>672.30082786821572</v>
+      </c>
+      <c r="J3">
+        <f>D3 * 2 * PI()</f>
+        <v>1227.1060904921733</v>
+      </c>
+      <c r="K3">
+        <f>E3 * 2 * PI()</f>
+        <v>86.079638708360349</v>
+      </c>
+      <c r="L3">
+        <f>F3 * 2 * PI()</f>
+        <v>100.53096491487338</v>
+      </c>
+      <c r="M3">
+        <f>G3 * 2 * PI()</f>
+        <v>29.530970943743984</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N11" si="3">SQRT(D3*D3+B3*B3-C3*C3)</f>
+        <v>186.43264199168559</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="4">N3*2*PI()</f>
+        <v>1171.3908369408309</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P5" si="5">$N$2-N3</f>
+        <v>2.2025880158609823</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q11" si="6">P3*2*PI()</f>
+        <v>13.839268659027562</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -540,8 +680,48 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
+      <c r="H4" t="e">
+        <f>B4 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I4" t="e">
+        <f>C4 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J4">
+        <f>D4 * 2 * PI()</f>
+        <v>1200.088393671301</v>
+      </c>
+      <c r="K4" t="e">
+        <f>E4 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L4" t="e">
+        <f>F4 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M4">
+        <f>G4 * 2 * PI()</f>
+        <v>56.548667764616276</v>
+      </c>
+      <c r="N4" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O4" t="e">
+        <f t="shared" si="4"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P4" t="e">
+        <f t="shared" si="5"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q4" t="e">
+        <f t="shared" si="6"/>
+        <v>#VALUE!</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -566,8 +746,48 @@
         <f t="shared" si="2"/>
         <v>17.199999999999989</v>
       </c>
+      <c r="H5">
+        <f>B5 * 2 * PI()</f>
+        <v>638.37162720944593</v>
+      </c>
+      <c r="I5">
+        <f>C5 * 2 * PI()</f>
+        <v>775.34506690596095</v>
+      </c>
+      <c r="J5">
+        <f>D5 * 2 * PI()</f>
+        <v>1148.5662741524284</v>
+      </c>
+      <c r="K5">
+        <f>E5 * 2 * PI()</f>
+        <v>11.938052083641249</v>
+      </c>
+      <c r="L5">
+        <f>F5 * 2 * PI()</f>
+        <v>-2.51327412287187</v>
+      </c>
+      <c r="M5">
+        <f>G5 * 2 * PI()</f>
+        <v>108.07078728348881</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>168.85153241827567</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="4"/>
+        <v>1060.9254675852674</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="5"/>
+        <v>19.783697589270901</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="6"/>
+        <v>124.30463801459112</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>0</v>
       </c>
@@ -586,8 +806,26 @@
       <c r="G7" t="s">
         <v>7</v>
       </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -605,15 +843,55 @@
         <v>0</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:G8" si="3">C$8-C8</f>
+        <f t="shared" ref="F8:G8" si="7">C$8-C8</f>
         <v>0</v>
       </c>
       <c r="G8">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>B8 * 2 * PI()</f>
+        <v>1719.079500044335</v>
+      </c>
+      <c r="I8">
+        <f>C8 * 2 * PI()</f>
+        <v>2038.2653136490576</v>
+      </c>
+      <c r="J8">
+        <f>D8 * 2 * PI()</f>
+        <v>2692.3449041264525</v>
+      </c>
+      <c r="K8">
+        <f>E8 * 2 * PI()</f>
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <f>F8 * 2 * PI()</f>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <f>G8 * 2 * PI()</f>
+        <v>0</v>
+      </c>
+      <c r="N8">
         <f t="shared" si="3"/>
+        <v>391.45095478233287</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="4"/>
+        <v>2459.5588875697745</v>
+      </c>
+      <c r="P8">
+        <f>$N$8-N8</f>
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -627,19 +905,59 @@
         <v>418.9</v>
       </c>
       <c r="E9">
-        <f t="shared" ref="E9:E11" si="4">B$8-B9</f>
+        <f t="shared" ref="E9:E11" si="8">B$8-B9</f>
         <v>54.600000000000023</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F11" si="5">C$8-C9</f>
+        <f t="shared" ref="F9:F11" si="9">C$8-C9</f>
         <v>17.799999999999955</v>
       </c>
       <c r="G9">
-        <f t="shared" ref="G9:G11" si="6">D$8-D9</f>
+        <f t="shared" ref="G9:G11" si="10">D$8-D9</f>
         <v>9.6000000000000227</v>
       </c>
+      <c r="H9">
+        <f>B9 * 2 * PI()</f>
+        <v>1376.0175822723295</v>
+      </c>
+      <c r="I9">
+        <f>C9 * 2 * PI()</f>
+        <v>1926.4246151812613</v>
+      </c>
+      <c r="J9">
+        <f>D9 * 2 * PI()</f>
+        <v>2632.0263251775286</v>
+      </c>
+      <c r="K9">
+        <f>E9 * 2 * PI()</f>
+        <v>343.06191777200553</v>
+      </c>
+      <c r="L9">
+        <f>F9 * 2 * PI()</f>
+        <v>111.84069846779634</v>
+      </c>
+      <c r="M9">
+        <f>G9 * 2 * PI()</f>
+        <v>60.31857894892417</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>359.77027392490334</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="4"/>
+        <v>2260.5032990849277</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ref="P9:P11" si="11">$N$2-N9</f>
+        <v>-171.13504391735677</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="6"/>
+        <v>-1075.2731934850692</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -653,19 +971,59 @@
         <v>412.5</v>
       </c>
       <c r="E10" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F10" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="10"/>
+        <v>16</v>
+      </c>
+      <c r="H10" t="e">
+        <f>B10 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I10" t="e">
+        <f>C10 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="J10">
+        <f>D10 * 2 * PI()</f>
+        <v>2591.8139392115795</v>
+      </c>
+      <c r="K10" t="e">
+        <f>E10 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="L10" t="e">
+        <f>F10 * 2 * PI()</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M10">
+        <f>G10 * 2 * PI()</f>
+        <v>100.53096491487338</v>
+      </c>
+      <c r="N10" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="O10" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="F10" t="e">
-        <f t="shared" si="5"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G10">
+      <c r="P10" t="e">
+        <f t="shared" si="11"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="Q10" t="e">
         <f t="shared" si="6"/>
-        <v>16</v>
+        <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -679,16 +1037,56 @@
         <v>393.4</v>
       </c>
       <c r="E11">
+        <f t="shared" si="8"/>
+        <v>5.6000000000000227</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="9"/>
+        <v>-7.2000000000000455</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="10"/>
+        <v>35.100000000000023</v>
+      </c>
+      <c r="H11">
+        <f>B11 * 2 * PI()</f>
+        <v>1683.8936623241291</v>
+      </c>
+      <c r="I11">
+        <f>C11 * 2 * PI()</f>
+        <v>2083.5042478607511</v>
+      </c>
+      <c r="J11">
+        <f>D11 * 2 * PI()</f>
+        <v>2471.8050998444492</v>
+      </c>
+      <c r="K11">
+        <f>E11 * 2 * PI()</f>
+        <v>35.185837720205825</v>
+      </c>
+      <c r="L11">
+        <f>F11 * 2 * PI()</f>
+        <v>-45.238934211693305</v>
+      </c>
+      <c r="M11">
+        <f>G11 * 2 * PI()</f>
+        <v>220.53980428200362</v>
+      </c>
+      <c r="N11">
+        <f t="shared" si="3"/>
+        <v>341.50988272669349</v>
+      </c>
+      <c r="O11">
         <f t="shared" si="4"/>
-        <v>5.6000000000000227</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="5"/>
-        <v>-7.2000000000000455</v>
-      </c>
-      <c r="G11">
+        <v>2145.7698774049841</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="11"/>
+        <v>-152.87465271914692</v>
+      </c>
+      <c r="Q11">
         <f t="shared" si="6"/>
-        <v>35.100000000000023</v>
+        <v>-960.53977180512572</v>
       </c>
     </row>
   </sheetData>

</xml_diff>